<commit_message>
Actualización de bitácora de incidencias y cronograma
</commit_message>
<xml_diff>
--- a/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Bitácora de incidencias.xlsx
+++ b/WebSecurity/DESARROLLO/PWCEV/Documentos/PWCEV-Bitácora de incidencias.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Project\WebSecurity\WebSecurity\DESARROLLO\PWCEV\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E309D6E9-2808-4331-9E25-66D552B4541B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73F89A5-4DD2-4180-B830-F94CCA332231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22227A93-5020-46C7-8FA6-1374034E3F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>N° incidencia</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
     <t>Cambio de direcciones de correo electrónico acorde al dominio de la universidad Nacional Mayor de San Marcos, adicional a ello debe ser String.</t>
   </si>
   <si>
@@ -88,6 +85,15 @@
   </si>
   <si>
     <t xml:space="preserve">Depuración de roles (Solo alumno y profesor), eliminar administrador </t>
+  </si>
+  <si>
+    <t>Corrección del ingreso de datos para el registro de exámenes</t>
+  </si>
+  <si>
+    <t>Asignación de alternativas a cada pregunta creada por examen según su orden y cantidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend </t>
   </si>
 </sst>
 </file>
@@ -152,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -171,12 +177,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DAD214-DB60-4883-8FB1-1E1EC2BCC74C}">
   <dimension ref="B3:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,12 +506,12 @@
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -538,13 +538,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -554,13 +554,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -570,13 +570,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -586,13 +586,13 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -602,13 +602,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -618,13 +618,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -634,13 +634,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -650,13 +650,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -666,13 +666,13 @@
         <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -682,23 +682,42 @@
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>11</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>